<commit_message>
Updated the meta data indicator
</commit_message>
<xml_diff>
--- a/nlp/sample_25rows.xlsx
+++ b/nlp/sample_25rows.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahz/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lidan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8F4C5CB-7F14-D840-88CC-CA4BBD5123FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1460A78-24BA-054F-B01E-AA63278621D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="500" windowWidth="26840" windowHeight="14600" xr2:uid="{B2EA32BF-59E3-A246-9269-E89DCE0866A4}"/>
+    <workbookView xWindow="0" yWindow="8000" windowWidth="25600" windowHeight="14600" xr2:uid="{B2EA32BF-59E3-A246-9269-E89DCE0866A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="127">
   <si>
     <t>indicator</t>
   </si>
@@ -344,6 +344,75 @@
   </si>
   <si>
     <t>meta_data</t>
+  </si>
+  <si>
+    <t>3.5, 11.2</t>
+  </si>
+  <si>
+    <t>1.2.1, 10.1.1,10.2.1</t>
+  </si>
+  <si>
+    <t>3.8.1,3.8.2,1.a.2</t>
+  </si>
+  <si>
+    <t>2.1.2,2.2.1,2.2.2,2.2.3</t>
+  </si>
+  <si>
+    <t>3.1, 3.2, 3.8</t>
+  </si>
+  <si>
+    <t>4.5, 5.b, 8.5, 8.6, 8.b, 9.2, 9.c</t>
+  </si>
+  <si>
+    <t>12.8,13.3</t>
+  </si>
+  <si>
+    <t>5.2.2, 11.7.2, 16.1.3, 16.2.3</t>
+  </si>
+  <si>
+    <t>16.7.1</t>
+  </si>
+  <si>
+    <t>6.3.2, 6.4.1, 6.4.2, 6.5.1, 6.5.2, 15.3.1</t>
+  </si>
+  <si>
+    <t>3.9.1</t>
+  </si>
+  <si>
+    <t>any economic statistics related SDG indicator</t>
+  </si>
+  <si>
+    <t>9.3.2</t>
+  </si>
+  <si>
+    <t>1.1.1, 1.2.1, 10.2.1</t>
+  </si>
+  <si>
+    <t>11.3.1, 11.7.1, 9.1.1</t>
+  </si>
+  <si>
+    <t>11.2.1, 11.6.2, 11.7.1, 11.a.1, 15.1.2, 11.7.2, 11.b.1</t>
+  </si>
+  <si>
+    <t>4.7, 13.3</t>
+  </si>
+  <si>
+    <t>4.7, 12.8</t>
+  </si>
+  <si>
+    <t>14.7.1</t>
+  </si>
+  <si>
+    <t>15.2.1</t>
+  </si>
+  <si>
+    <t>14.5.1, 15.1.2</t>
+  </si>
+  <si>
+    <t>16.1.1, 16.1.3, 16.1.4, 16.4.2, 16.a.1, 10.3.1, 16.b.1, 5.2.2</t>
+  </si>
+  <si>
+    <t>17.1.2</t>
   </si>
 </sst>
 </file>
@@ -746,7 +815,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -786,6 +855,9 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -800,6 +872,9 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
+      <c r="E3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -814,6 +889,9 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
+      <c r="E4" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -828,6 +906,9 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
+      <c r="E5" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -842,6 +923,9 @@
       <c r="D6" t="s">
         <v>23</v>
       </c>
+      <c r="E6" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -856,6 +940,9 @@
       <c r="D7" t="s">
         <v>27</v>
       </c>
+      <c r="E7" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -870,6 +957,9 @@
       <c r="D8" t="s">
         <v>31</v>
       </c>
+      <c r="E8" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -884,6 +974,9 @@
       <c r="D9" t="s">
         <v>35</v>
       </c>
+      <c r="E9" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -898,6 +991,9 @@
       <c r="D10" t="s">
         <v>39</v>
       </c>
+      <c r="E10" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -912,6 +1008,9 @@
       <c r="D11" t="s">
         <v>43</v>
       </c>
+      <c r="E11" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -926,6 +1025,9 @@
       <c r="D12" t="s">
         <v>47</v>
       </c>
+      <c r="E12" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -940,6 +1042,9 @@
       <c r="D13" t="s">
         <v>51</v>
       </c>
+      <c r="E13" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -954,6 +1059,9 @@
       <c r="D14" t="s">
         <v>55</v>
       </c>
+      <c r="E14" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -968,6 +1076,9 @@
       <c r="D15" t="s">
         <v>59</v>
       </c>
+      <c r="E15" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -982,8 +1093,11 @@
       <c r="D16" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>64</v>
       </c>
@@ -996,8 +1110,11 @@
       <c r="D17" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>68</v>
       </c>
@@ -1010,8 +1127,11 @@
       <c r="D18" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>72</v>
       </c>
@@ -1024,8 +1144,11 @@
       <c r="D19" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>76</v>
       </c>
@@ -1038,8 +1161,11 @@
       <c r="D20" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>80</v>
       </c>
@@ -1052,8 +1178,11 @@
       <c r="D21" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>83</v>
       </c>
@@ -1066,8 +1195,11 @@
       <c r="D22" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>87</v>
       </c>
@@ -1080,8 +1212,11 @@
       <c r="D23" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>91</v>
       </c>
@@ -1094,8 +1229,11 @@
       <c r="D24" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>95</v>
       </c>
@@ -1108,8 +1246,11 @@
       <c r="D25" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>99</v>
       </c>
@@ -1121,6 +1262,9 @@
       </c>
       <c r="D26" s="2" t="s">
         <v>102</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>